<commit_message>
Draft design specification v1.0
</commit_message>
<xml_diff>
--- a/PCB/04 Dev_Lib/4.2_Design/SystemArchitecture-Clay-v1.0.xlsx
+++ b/PCB/04 Dev_Lib/4.2_Design/SystemArchitecture-Clay-v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram View" sheetId="2" r:id="rId1"/>
@@ -75,84 +75,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>550334</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>127003</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>105838</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10456334" y="2032003"/>
-          <a:ext cx="5228166" cy="4847168"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1"/>
-            <a:t>Web Server</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1"/>
-            <a:t>Apache</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
-            <a:t> 7.1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>67734</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>12693</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>309034</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>50793</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -161,8 +93,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2544234" y="12693"/>
-          <a:ext cx="4368800" cy="4483100"/>
+          <a:off x="2544234" y="482601"/>
+          <a:ext cx="4368800" cy="4305300"/>
           <a:chOff x="3263900" y="1435100"/>
           <a:chExt cx="4368800" cy="4305300"/>
         </a:xfrm>
@@ -588,14 +520,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>491069</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114308</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>287869</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>101601</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>165108</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -604,8 +536,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7095069" y="3225800"/>
-          <a:ext cx="3098800" cy="1744134"/>
+          <a:off x="7095069" y="3568708"/>
+          <a:ext cx="3098800" cy="1676400"/>
           <a:chOff x="8026400" y="7471833"/>
           <a:chExt cx="3098800" cy="1731434"/>
         </a:xfrm>
@@ -692,7 +624,7 @@
             <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="en-US" sz="2400" b="1"/>
-              <a:t>HTTP</a:t>
+              <a:t>HTTP Request</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -704,14 +636,14 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>148171</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>169337</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>21178</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -720,7 +652,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17868900" y="2688171"/>
+          <a:off x="17868900" y="3175012"/>
           <a:ext cx="2311400" cy="3196166"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
@@ -778,96 +710,386 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>173566</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>550334</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>8</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>414866</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>190509</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="Group 4"/>
+        <xdr:cNvPr id="12" name="Group 11"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10905066" y="2802467"/>
-          <a:ext cx="4368800" cy="3462867"/>
-          <a:chOff x="10905066" y="2802467"/>
-          <a:chExt cx="4368800" cy="3462867"/>
+          <a:off x="10456334" y="2235208"/>
+          <a:ext cx="5228166" cy="4660901"/>
+          <a:chOff x="10456334" y="2328341"/>
+          <a:chExt cx="5228166" cy="4847168"/>
         </a:xfrm>
       </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10456334" y="2328341"/>
+            <a:ext cx="5228166" cy="4847168"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Web Server</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Apache</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t> 7.1</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="29" name="Group 28"/>
+          <xdr:cNvPr id="5" name="Group 4"/>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="10905066" y="2802467"/>
+            <a:off x="10905066" y="3289308"/>
             <a:ext cx="4368800" cy="3462867"/>
-            <a:chOff x="9656233" y="2273300"/>
+            <a:chOff x="10905066" y="2802467"/>
             <a:chExt cx="4368800" cy="3462867"/>
           </a:xfrm>
         </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="29" name="Group 28"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="10905066" y="2802467"/>
+              <a:ext cx="4368800" cy="3462867"/>
+              <a:chOff x="9656233" y="2273300"/>
+              <a:chExt cx="4368800" cy="3462867"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="19" name="Rectangle 18"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="9656233" y="2273300"/>
+                <a:ext cx="4368800" cy="3462867"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
+                  <a:t>Controller</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="20" name="Rounded Rectangle 19"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10879666" y="2781300"/>
+                <a:ext cx="2794000" cy="436033"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Story</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> controller</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="21" name="Rounded Rectangle 20"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10879666" y="3302000"/>
+                <a:ext cx="2794000" cy="436033"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Course controller</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="22" name="Rounded Rectangle 21"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="10879666" y="3814233"/>
+                <a:ext cx="2794000" cy="436033"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>User </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>controller</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="9952566" y="2747434"/>
+                <a:ext cx="596900" cy="2650066"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert" rtlCol="0" anchor="ctr"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
+                  <a:t>Web Service API</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="Rectangle 18"/>
+            <xdr:cNvPr id="27" name="Rounded Rectangle 26"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9656233" y="2273300"/>
-              <a:ext cx="4368800" cy="3462867"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="tx2"/>
-            </a:solidFill>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="2000" b="1"/>
-                <a:t>Controller</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="20" name="Rounded Rectangle 19"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10879666" y="2781300"/>
+              <a:off x="12132732" y="4855633"/>
               <a:ext cx="2794000" cy="436033"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -899,136 +1121,12 @@
             <a:p>
               <a:pPr algn="l"/>
               <a:r>
-                <a:rPr lang="en-US" sz="1600">
+                <a:rPr lang="en-US" sz="1600" b="0" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="bg1"/>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Story</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="bg1"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t> controller</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1600">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="21" name="Rounded Rectangle 20"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10879666" y="3302000"/>
-              <a:ext cx="2794000" cy="436033"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="bg1"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>Course controller</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1600">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="22" name="Rounded Rectangle 21"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="10879666" y="3814233"/>
-              <a:ext cx="2794000" cy="436033"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="bg1"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>User </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="bg1"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>controller</a:t>
+                <a:t>Authentication</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1600" b="1">
                 <a:solidFill>
@@ -1038,106 +1136,7 @@
             </a:p>
           </xdr:txBody>
         </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9952566" y="2747434"/>
-              <a:ext cx="596900" cy="2650066"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-US" sz="2400" b="1"/>
-                <a:t>Web Service API</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
       </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="27" name="Rounded Rectangle 26"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="12132732" y="4855633"/>
-            <a:ext cx="2794000" cy="436033"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Authentication</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1145,14 +1144,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>105833</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>8469</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>402167</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>33870</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>97377</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1161,7 +1160,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15790333" y="4030136"/>
+          <a:off x="15790333" y="4516977"/>
           <a:ext cx="1947334" cy="872067"/>
         </a:xfrm>
         <a:prstGeom prst="leftRightArrow">
@@ -1202,14 +1201,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>71967</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>143926</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>207434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>313267</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>182026</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1218,8 +1217,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2548467" y="4588926"/>
-          <a:ext cx="4368800" cy="4483100"/>
+          <a:off x="2548467" y="4881034"/>
+          <a:ext cx="4368800" cy="4296833"/>
           <a:chOff x="3263900" y="1435100"/>
           <a:chExt cx="4368800" cy="4305300"/>
         </a:xfrm>
@@ -1588,8 +1587,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9364071" y="4018887"/>
-          <a:ext cx="7544368" cy="1510352"/>
+          <a:off x="9270243" y="3978370"/>
+          <a:ext cx="7467599" cy="1495425"/>
           <a:chOff x="1706160" y="4037842"/>
           <a:chExt cx="7544368" cy="1510352"/>
         </a:xfrm>
@@ -1764,8 +1763,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9364260" y="885019"/>
-          <a:ext cx="7544368" cy="1510352"/>
+          <a:off x="9270432" y="876489"/>
+          <a:ext cx="7467599" cy="1495425"/>
           <a:chOff x="1744260" y="7178154"/>
           <a:chExt cx="7544368" cy="1510352"/>
         </a:xfrm>
@@ -2062,8 +2061,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9370515" y="2446172"/>
-          <a:ext cx="7544368" cy="1515660"/>
+          <a:off x="9276687" y="2422715"/>
+          <a:ext cx="7467599" cy="1498600"/>
           <a:chOff x="1731560" y="5611694"/>
           <a:chExt cx="7544368" cy="1515660"/>
         </a:xfrm>
@@ -2365,8 +2364,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9408237" y="5598994"/>
-          <a:ext cx="7544368" cy="1515660"/>
+          <a:off x="9314409" y="5543550"/>
+          <a:ext cx="7467599" cy="1498600"/>
           <a:chOff x="1693460" y="2471382"/>
           <a:chExt cx="7544368" cy="1515660"/>
         </a:xfrm>
@@ -2582,8 +2581,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9395536" y="7165454"/>
-          <a:ext cx="7544368" cy="1510352"/>
+          <a:off x="9301708" y="7092950"/>
+          <a:ext cx="7467599" cy="1495425"/>
           <a:chOff x="1680760" y="891275"/>
           <a:chExt cx="7544368" cy="1510352"/>
         </a:xfrm>
@@ -2960,8 +2959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2975,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" topLeftCell="A2" zoomScale="67" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="E3" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>